<commit_message>
fixed projection, 180 overlap issue remaining
</commit_message>
<xml_diff>
--- a/material/angles.xlsx
+++ b/material/angles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richard/Developer/laptime/material/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{127CE3BD-2555-BC4A-B1ED-95C7D7213200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0CBB597-FE07-5C47-B3C8-6AAEB9851FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16500" activeTab="1" xr2:uid="{DF8CADEB-DD68-B34F-8C7A-18C404D9E686}"/>
   </bookViews>
@@ -318,17 +318,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -957,7 +947,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -972,7 +962,7 @@
         <v>24</v>
       </c>
       <c r="B1" s="16">
-        <v>2</v>
+        <v>-2</v>
       </c>
       <c r="D1" t="s">
         <v>29</v>
@@ -990,7 +980,7 @@
         <v>25</v>
       </c>
       <c r="B2" s="16">
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E2" t="s">
         <v>31</v>
@@ -1028,12 +1018,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$B$3/2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>